<commit_message>
updated results from slr
</commit_message>
<xml_diff>
--- a/domainphasesslr.xlsx
+++ b/domainphasesslr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugoa\Desktop\repos\slrdevopsmde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D327FA5-D54F-41C4-817C-E1E757F050A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB6587F-023C-4496-96D2-56E1FBC7D08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{52FB02F0-5B6D-4E3B-9C4E-7F5F7E4C1247}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>Paper</t>
   </si>
@@ -410,6 +410,21 @@
   </si>
   <si>
     <t>Towards LowDevSecOps Framework for Low-Code Development: Integrating Process-Oriented Recommendations for Security Risk Management</t>
+  </si>
+  <si>
+    <t>A Model-Driven Approach for Systematic Reproducibility and Replicability of Data Science Projects</t>
+  </si>
+  <si>
+    <t>Industrial requirements for supporting AI-enhanced model-driven engineering</t>
+  </si>
+  <si>
+    <t>MDE for machine learning-enabled software systems: a case study and comparison of MontiAnna &amp;amp; ML-Quadrat</t>
+  </si>
+  <si>
+    <t>Model-based fleet deployment in the IoT–edge–cloud continuum</t>
+  </si>
+  <si>
+    <t>AI-augmented Model-Based Capabilities in the AIDOaRt Project: Continuous Development of Cyber-Physical Systems</t>
   </si>
 </sst>
 </file>
@@ -470,7 +485,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +516,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -514,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -542,6 +569,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DA6E6E-EF9C-4888-81A2-98C57B59DF73}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,107 +1531,132 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>103</v>
+      <c r="A32" s="15" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>108</v>
+      <c r="A37" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>114</v>
+      <c r="A43" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>119</v>
+      <c r="A48" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1610,6 +1666,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="417546b7-7497-41cb-8a8a-51c855da4585" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010079FCC2D86B3A1C4D9D534683D06266FC" ma:contentTypeVersion="6" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="b78773f717836d3c2971633886dd9e3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="417546b7-7497-41cb-8a8a-51c855da4585" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0eb66bf715d8234ce9b68a294e2fbe0e" ns3:_="">
     <xsd:import namespace="417546b7-7497-41cb-8a8a-51c855da4585"/>
@@ -1765,37 +1838,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="417546b7-7497-41cb-8a8a-51c855da4585" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21FB5851-0DCF-4D31-87B2-A49C65FCCE88}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008E0A22-D167-41A5-B27F-152884A0B99F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="417546b7-7497-41cb-8a8a-51c855da4585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1817,9 +1863,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008E0A22-D167-41A5-B27F-152884A0B99F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21FB5851-0DCF-4D31-87B2-A49C65FCCE88}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="417546b7-7497-41cb-8a8a-51c855da4585"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>